<commit_message>
updates from Oct 12th
</commit_message>
<xml_diff>
--- a/reference_data/list_donors_categories.xlsx
+++ b/reference_data/list_donors_categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositaries\1.work\ERP\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980A82CA-D24A-4032-9C24-72B307EB031A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30333BA6-93F7-4750-8246-A5A295C9407F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>Donor</t>
   </si>
@@ -146,16 +146,32 @@
   </si>
   <si>
     <t>People's Postcode Lottery</t>
+  </si>
+  <si>
+    <t>Combination</t>
+  </si>
+  <si>
+    <t>Embassy of Sweden</t>
+  </si>
+  <si>
+    <t>Latter-Day St Charities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,8 +197,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,9 +496,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -741,39 +760,76 @@
       <c r="A32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>